<commit_message>
change in processed data sheets
</commit_message>
<xml_diff>
--- a/Statistik/Statistik_Python/SORTstatistics.xlsx
+++ b/Statistik/Statistik_Python/SORTstatistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten_Noah\Desktop_Dateien\Studium_Freiberg\Study\Semester 7\Bachelorarbeit\for Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thraco123\Documents\GitHub\Bachelorarbeit_PV-Anlagen\Statistik\Statistik_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C394E6D1-0A4F-4C68-BA10-8E3973064A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EE898F-2FA8-47A6-8A30-32B0F59A3BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6165" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6165" windowWidth="16440" windowHeight="29040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShinozakiSORT - Anlage" sheetId="7" r:id="rId1"/>
@@ -68,7 +68,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +86,12 @@
     </font>
     <font>
       <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -111,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -121,6 +127,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -403,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABBAE1-A925-4DA0-BED4-89746AE7853F}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,167 +442,167 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>14048</v>
       </c>
       <c r="C4" s="2">
         <v>9600</v>
       </c>
-      <c r="D4" s="2">
-        <v>13500</v>
+      <c r="D4" s="5">
+        <v>13667</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>20767</v>
+      <c r="B5" s="5">
+        <v>20757</v>
       </c>
       <c r="C5" s="2">
         <v>13590</v>
       </c>
-      <c r="D5" s="2">
-        <v>20864</v>
+      <c r="D5" s="5">
+        <v>21152</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
-        <v>24985</v>
+      <c r="B6" s="5">
+        <v>24957</v>
       </c>
       <c r="C6" s="2">
         <v>16481</v>
       </c>
-      <c r="D6" s="2">
-        <v>26041</v>
+      <c r="D6" s="5">
+        <v>26409</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <v>28059</v>
+      <c r="B7" s="5">
+        <v>28005</v>
       </c>
       <c r="C7" s="2">
         <v>18925</v>
       </c>
-      <c r="D7" s="2">
-        <v>30004</v>
+      <c r="D7" s="5">
+        <v>30416</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <v>30498</v>
+      <c r="B8" s="5">
+        <v>30410</v>
       </c>
       <c r="C8" s="2">
         <v>21092</v>
       </c>
-      <c r="D8" s="2">
-        <v>33192</v>
+      <c r="D8" s="5">
+        <v>33616</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
-        <v>32537</v>
+      <c r="B9" s="5">
+        <v>32410</v>
       </c>
       <c r="C9" s="2">
         <v>23040</v>
       </c>
-      <c r="D9" s="2">
-        <v>35847</v>
+      <c r="D9" s="5">
+        <v>36256</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
-        <v>34301</v>
+      <c r="B10" s="5">
+        <v>34127</v>
       </c>
       <c r="C10" s="2">
         <v>24800</v>
       </c>
-      <c r="D10" s="2">
-        <v>38114</v>
+      <c r="D10" s="5">
+        <v>38485</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="2">
-        <v>35863</v>
+      <c r="B11" s="5">
+        <v>35639</v>
       </c>
       <c r="C11" s="2">
         <v>26390</v>
       </c>
-      <c r="D11" s="2">
-        <v>40083</v>
+      <c r="D11" s="5">
+        <v>40398</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
-        <v>37271</v>
+      <c r="B12" s="5">
+        <v>36992</v>
       </c>
       <c r="C12" s="2">
         <v>27826</v>
       </c>
-      <c r="D12" s="2">
-        <v>41818</v>
+      <c r="D12" s="5">
+        <v>42064</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
-        <v>38559</v>
+      <c r="B13" s="5">
+        <v>38220</v>
       </c>
       <c r="C13" s="2">
         <v>29125</v>
       </c>
-      <c r="D13" s="2">
-        <v>43364</v>
+      <c r="D13" s="5">
+        <v>43530</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
-        <v>39750</v>
+      <c r="B14" s="5">
+        <v>39350</v>
       </c>
       <c r="C14" s="2">
         <v>30298</v>
       </c>
-      <c r="D14" s="2">
-        <v>44750</v>
+      <c r="D14" s="5">
+        <v>44833</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
-        <v>40862</v>
+      <c r="B15" s="5">
+        <v>40399</v>
       </c>
       <c r="C15" s="2">
         <v>31360</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="5">
         <v>46000</v>
       </c>
     </row>
@@ -603,8 +610,8 @@
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
-        <v>41911</v>
+      <c r="B16" s="5">
+        <v>41383</v>
       </c>
       <c r="C16" s="2">
         <v>32324</v>
@@ -614,8 +621,8 @@
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
-        <v>42907</v>
+      <c r="B17" s="5">
+        <v>42314</v>
       </c>
       <c r="C17" s="2">
         <v>33200</v>
@@ -625,8 +632,8 @@
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
-        <v>43860</v>
+      <c r="B18" s="5">
+        <v>43202</v>
       </c>
       <c r="C18" s="2">
         <v>34000</v>
@@ -636,48 +643,48 @@
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
-        <v>44777</v>
+      <c r="B19" s="5">
+        <v>44055</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="2">
-        <v>45664</v>
+      <c r="B20" s="5">
+        <v>44880</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="2">
-        <v>46526</v>
+      <c r="B21" s="5">
+        <v>45682</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="2">
-        <v>47367</v>
+      <c r="B22" s="5">
+        <v>46467</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="2">
-        <v>48190</v>
+      <c r="B23" s="5">
+        <v>47238</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="2">
-        <v>49000</v>
+      <c r="B24" s="5">
+        <v>48000</v>
       </c>
     </row>
   </sheetData>
@@ -689,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7C92C2-B345-4DAA-AA38-51369A0BF7AE}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +718,7 @@
       </c>
       <c r="B2" s="4">
         <f>B24/B4</f>
-        <v>3.4880410022779045</v>
+        <v>3.416856492027335</v>
       </c>
       <c r="C2" s="4">
         <f>C18/C4</f>
@@ -719,7 +726,7 @@
       </c>
       <c r="D2" s="4">
         <f>D15/D4</f>
-        <v>3.4074074074074074</v>
+        <v>3.3657715665471573</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -753,7 +760,7 @@
       </c>
       <c r="D4" s="3">
         <f>'ShinozakiSORT - Anlage'!D4/1000</f>
-        <v>13.5</v>
+        <v>13.667</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -762,7 +769,7 @@
       </c>
       <c r="B5" s="3">
         <f>'ShinozakiSORT - Anlage'!B5/1000</f>
-        <v>20.766999999999999</v>
+        <v>20.757000000000001</v>
       </c>
       <c r="C5" s="3">
         <f>'ShinozakiSORT - Anlage'!C5/1000</f>
@@ -770,7 +777,7 @@
       </c>
       <c r="D5" s="3">
         <f>'ShinozakiSORT - Anlage'!D5/1000</f>
-        <v>20.864000000000001</v>
+        <v>21.152000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -779,7 +786,7 @@
       </c>
       <c r="B6" s="3">
         <f>'ShinozakiSORT - Anlage'!B6/1000</f>
-        <v>24.984999999999999</v>
+        <v>24.957000000000001</v>
       </c>
       <c r="C6" s="3">
         <f>'ShinozakiSORT - Anlage'!C6/1000</f>
@@ -787,7 +794,7 @@
       </c>
       <c r="D6" s="3">
         <f>'ShinozakiSORT - Anlage'!D6/1000</f>
-        <v>26.041</v>
+        <v>26.408999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -796,7 +803,7 @@
       </c>
       <c r="B7" s="3">
         <f>'ShinozakiSORT - Anlage'!B7/1000</f>
-        <v>28.059000000000001</v>
+        <v>28.004999999999999</v>
       </c>
       <c r="C7" s="3">
         <f>'ShinozakiSORT - Anlage'!C7/1000</f>
@@ -804,7 +811,7 @@
       </c>
       <c r="D7" s="3">
         <f>'ShinozakiSORT - Anlage'!D7/1000</f>
-        <v>30.004000000000001</v>
+        <v>30.416</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -813,7 +820,7 @@
       </c>
       <c r="B8" s="3">
         <f>'ShinozakiSORT - Anlage'!B8/1000</f>
-        <v>30.498000000000001</v>
+        <v>30.41</v>
       </c>
       <c r="C8" s="3">
         <f>'ShinozakiSORT - Anlage'!C8/1000</f>
@@ -821,7 +828,7 @@
       </c>
       <c r="D8" s="3">
         <f>'ShinozakiSORT - Anlage'!D8/1000</f>
-        <v>33.192</v>
+        <v>33.616</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -830,7 +837,7 @@
       </c>
       <c r="B9" s="3">
         <f>'ShinozakiSORT - Anlage'!B9/1000</f>
-        <v>32.536999999999999</v>
+        <v>32.409999999999997</v>
       </c>
       <c r="C9" s="3">
         <f>'ShinozakiSORT - Anlage'!C9/1000</f>
@@ -838,7 +845,7 @@
       </c>
       <c r="D9" s="3">
         <f>'ShinozakiSORT - Anlage'!D9/1000</f>
-        <v>35.847000000000001</v>
+        <v>36.256</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -847,7 +854,7 @@
       </c>
       <c r="B10" s="3">
         <f>'ShinozakiSORT - Anlage'!B10/1000</f>
-        <v>34.301000000000002</v>
+        <v>34.127000000000002</v>
       </c>
       <c r="C10" s="3">
         <f>'ShinozakiSORT - Anlage'!C10/1000</f>
@@ -855,7 +862,7 @@
       </c>
       <c r="D10" s="3">
         <f>'ShinozakiSORT - Anlage'!D10/1000</f>
-        <v>38.113999999999997</v>
+        <v>38.484999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -864,7 +871,7 @@
       </c>
       <c r="B11" s="3">
         <f>'ShinozakiSORT - Anlage'!B11/1000</f>
-        <v>35.863</v>
+        <v>35.639000000000003</v>
       </c>
       <c r="C11" s="3">
         <f>'ShinozakiSORT - Anlage'!C11/1000</f>
@@ -872,7 +879,7 @@
       </c>
       <c r="D11" s="3">
         <f>'ShinozakiSORT - Anlage'!D11/1000</f>
-        <v>40.082999999999998</v>
+        <v>40.398000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,7 +888,7 @@
       </c>
       <c r="B12" s="3">
         <f>'ShinozakiSORT - Anlage'!B12/1000</f>
-        <v>37.271000000000001</v>
+        <v>36.991999999999997</v>
       </c>
       <c r="C12" s="3">
         <f>'ShinozakiSORT - Anlage'!C12/1000</f>
@@ -889,7 +896,7 @@
       </c>
       <c r="D12" s="3">
         <f>'ShinozakiSORT - Anlage'!D12/1000</f>
-        <v>41.817999999999998</v>
+        <v>42.064</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -898,7 +905,7 @@
       </c>
       <c r="B13" s="3">
         <f>'ShinozakiSORT - Anlage'!B13/1000</f>
-        <v>38.558999999999997</v>
+        <v>38.22</v>
       </c>
       <c r="C13" s="3">
         <f>'ShinozakiSORT - Anlage'!C13/1000</f>
@@ -906,7 +913,7 @@
       </c>
       <c r="D13" s="3">
         <f>'ShinozakiSORT - Anlage'!D13/1000</f>
-        <v>43.363999999999997</v>
+        <v>43.53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,7 +922,7 @@
       </c>
       <c r="B14" s="3">
         <f>'ShinozakiSORT - Anlage'!B14/1000</f>
-        <v>39.75</v>
+        <v>39.35</v>
       </c>
       <c r="C14" s="3">
         <f>'ShinozakiSORT - Anlage'!C14/1000</f>
@@ -923,7 +930,7 @@
       </c>
       <c r="D14" s="3">
         <f>'ShinozakiSORT - Anlage'!D14/1000</f>
-        <v>44.75</v>
+        <v>44.832999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -932,7 +939,7 @@
       </c>
       <c r="B15" s="3">
         <f>'ShinozakiSORT - Anlage'!B15/1000</f>
-        <v>40.862000000000002</v>
+        <v>40.399000000000001</v>
       </c>
       <c r="C15" s="3">
         <f>'ShinozakiSORT - Anlage'!C15/1000</f>
@@ -949,7 +956,7 @@
       </c>
       <c r="B16" s="3">
         <f>'ShinozakiSORT - Anlage'!B16/1000</f>
-        <v>41.911000000000001</v>
+        <v>41.383000000000003</v>
       </c>
       <c r="C16" s="3">
         <f>'ShinozakiSORT - Anlage'!C16/1000</f>
@@ -962,7 +969,7 @@
       </c>
       <c r="B17" s="3">
         <f>'ShinozakiSORT - Anlage'!B17/1000</f>
-        <v>42.906999999999996</v>
+        <v>42.314</v>
       </c>
       <c r="C17" s="3">
         <f>'ShinozakiSORT - Anlage'!C17/1000</f>
@@ -975,7 +982,7 @@
       </c>
       <c r="B18" s="3">
         <f>'ShinozakiSORT - Anlage'!B18/1000</f>
-        <v>43.86</v>
+        <v>43.201999999999998</v>
       </c>
       <c r="C18" s="3">
         <f>'ShinozakiSORT - Anlage'!C18/1000</f>
@@ -988,7 +995,7 @@
       </c>
       <c r="B19" s="3">
         <f>'ShinozakiSORT - Anlage'!B19/1000</f>
-        <v>44.777000000000001</v>
+        <v>44.055</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -997,7 +1004,7 @@
       </c>
       <c r="B20" s="3">
         <f>'ShinozakiSORT - Anlage'!B20/1000</f>
-        <v>45.664000000000001</v>
+        <v>44.88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,7 +1013,7 @@
       </c>
       <c r="B21" s="3">
         <f>'ShinozakiSORT - Anlage'!B21/1000</f>
-        <v>46.526000000000003</v>
+        <v>45.682000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,7 +1022,7 @@
       </c>
       <c r="B22" s="3">
         <f>'ShinozakiSORT - Anlage'!B22/1000</f>
-        <v>47.366999999999997</v>
+        <v>46.466999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1031,7 @@
       </c>
       <c r="B23" s="3">
         <f>'ShinozakiSORT - Anlage'!B23/1000</f>
-        <v>48.19</v>
+        <v>47.238</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,7 +1040,7 @@
       </c>
       <c r="B24" s="3">
         <f>'ShinozakiSORT - Anlage'!B24/1000</f>
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>